<commit_message>
update record to log file
</commit_message>
<xml_diff>
--- a/applications/VBA/logLine.xlsx
+++ b/applications/VBA/logLine.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\Linearity\applications\VBA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9182E8-3942-4BD2-A6C0-3A2AA64972F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="13890" yWindow="480" windowWidth="14910" windowHeight="14145" xr2:uid="{5B57F47A-673B-40C3-9873-C20F118C58A1}"/>
+    <workbookView xWindow="13890" yWindow="480" windowWidth="14910" windowHeight="14145"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>start application</t>
   </si>
@@ -55,26 +49,92 @@
     <t>port Multimetr</t>
   </si>
   <si>
+    <t>COM6</t>
+  </si>
+  <si>
+    <t>Function linkPort</t>
+  </si>
+  <si>
+    <t>open Port 1</t>
+  </si>
+  <si>
+    <t>COM6:9600,N,8,1</t>
+  </si>
+  <si>
+    <t>request as data and avswer port 1</t>
+  </si>
+  <si>
+    <t>*idn?   GW, GDM8255A, 1.0</t>
+  </si>
+  <si>
+    <t>if length &gt; 0</t>
+  </si>
+  <si>
+    <t>Function multimetrCorrect</t>
+  </si>
+  <si>
     <t>scan Ports</t>
   </si>
   <si>
-    <t>portsPro() length</t>
-  </si>
-  <si>
     <t>ports() length</t>
   </si>
   <si>
-    <t>working Port</t>
+    <t>checkPortsMassive</t>
+  </si>
+  <si>
+    <t>scan Port for A2</t>
   </si>
   <si>
     <t>COM1</t>
+  </si>
+  <si>
+    <t>open Port 2</t>
+  </si>
+  <si>
+    <t>COM1:9600,N,8,1</t>
+  </si>
+  <si>
+    <t>Function sendAngle: anglVar</t>
+  </si>
+  <si>
+    <t>hlo</t>
+  </si>
+  <si>
+    <t>result from Port 2</t>
+  </si>
+  <si>
+    <t>request as data and avswer port 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hlo   </t>
+  </si>
+  <si>
+    <t>else length &gt; 0</t>
+  </si>
+  <si>
+    <t>close Port 2</t>
+  </si>
+  <si>
+    <t>Function controlCorrect</t>
+  </si>
+  <si>
+    <t>portControl hlo = 25</t>
+  </si>
+  <si>
+    <t>end checkPortsMassive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COM6 </t>
+  </si>
+  <si>
+    <t>close Port 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,7 +233,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -225,7 +285,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -419,110 +479,830 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37352786-5EC9-4F6D-BE65-E6C7503A3D42}">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="3" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>0.58223379629629635</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3">
+        <v>0.59149305555555554</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>0.58224537037037039</v>
-      </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3">
+        <v>0.59151620370370372</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>0.58225694444444442</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="3">
+        <v>0.5915393518518518</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>0.58225694444444442</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="3">
+        <v>0.59155092592592595</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>0.58226851851851846</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="3">
+        <v>0.59157407407407414</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>0.58228009259259261</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="3">
-        <v>0.5823032407407408</v>
+        <v>0.59159722222222222</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="3">
-        <v>0.5823032407407408</v>
+        <v>0.59160879629629626</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="3">
-        <v>0.58231481481481484</v>
+        <v>0.59165509259259264</v>
       </c>
       <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3">
+        <v>0.59167824074074071</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3">
+        <v>0.59168981481481475</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3">
+        <v>0.59171296296296294</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3">
+        <v>0.59173611111111113</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3">
+        <v>0.59174768518518517</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3">
+        <v>0.59177083333333336</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="3">
+        <v>0.59179398148148155</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3">
+        <v>0.59181712962962962</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3">
+        <v>0.59185185185185185</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3">
+        <v>0.59187500000000004</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3">
+        <v>0.59188657407407408</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3">
+        <v>0.59190972222222216</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3">
+        <v>0.59193287037037035</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="3">
+        <v>0.59195601851851853</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3">
+        <v>0.59197916666666661</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="3">
+        <v>0.59199074074074076</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="3">
+        <v>0.59201388888888895</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="3">
+        <v>0.59203703703703703</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="3">
+        <v>0.59302083333333333</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="3">
+        <v>0.59304398148148152</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="3"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="3"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="3"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="3"/>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="3"/>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="3"/>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="3"/>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="3"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="3"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="3"/>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="3"/>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="3"/>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="3"/>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="3"/>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="3"/>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="3"/>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="3"/>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="3"/>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="3"/>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="3"/>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="3"/>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="3"/>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="3"/>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="3"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="3"/>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="3"/>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="3"/>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="3"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="3"/>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="3"/>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="3"/>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="3"/>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="3"/>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="3"/>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="3"/>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="3"/>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="3"/>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="3"/>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="3"/>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="3"/>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="3"/>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="3"/>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="3"/>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="3"/>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="3"/>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="3"/>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="3"/>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="3"/>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="3"/>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="3"/>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="3"/>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="3"/>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="3"/>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="3"/>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="3"/>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="3"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="3"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="3"/>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="3"/>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="3"/>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="3"/>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="3"/>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="3"/>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="3"/>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="3"/>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="3"/>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="3"/>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="3"/>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="3"/>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="3"/>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="3"/>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="3"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="3"/>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="3"/>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="3"/>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="3"/>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="3"/>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="3"/>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="3"/>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="3"/>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="3"/>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="3"/>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="3"/>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="3"/>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="3"/>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="3"/>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="3"/>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="3"/>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="3"/>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="3"/>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="3"/>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="3"/>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="3"/>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="3"/>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="3"/>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="3"/>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="3"/>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="3"/>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="3"/>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="3"/>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="3"/>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="3"/>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="3"/>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="3"/>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="3"/>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="3"/>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="3"/>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="3"/>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="3"/>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="3"/>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="3"/>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" s="3"/>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" s="3"/>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" s="3"/>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" s="3"/>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" s="3"/>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" s="3"/>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="3"/>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" s="3"/>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" s="3"/>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" s="3"/>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" s="3"/>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" s="3"/>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" s="3"/>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" s="3"/>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" s="3"/>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" s="3"/>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="3"/>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" s="3"/>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" s="3"/>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" s="3"/>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" s="3"/>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" s="3"/>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" s="3"/>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" s="3"/>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" s="3"/>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" s="3"/>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" s="3"/>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" s="3"/>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" s="3"/>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" s="3"/>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" s="3"/>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" s="3"/>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" s="3"/>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" s="3"/>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" s="3"/>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" s="3"/>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" s="3"/>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" s="3"/>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" s="3"/>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" s="3"/>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" s="3"/>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" s="3"/>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" s="3"/>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" s="3"/>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" s="3"/>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" s="3"/>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" s="3"/>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" s="3"/>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update scan and check ports in module1
</commit_message>
<xml_diff>
--- a/applications/VBA/logLine.xlsx
+++ b/applications/VBA/logLine.xlsx
@@ -1,32 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\Linearity\applications\VBA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED773AA-B3B7-4118-9DA8-AC9E4ED64F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13890" yWindow="480" windowWidth="14910" windowHeight="14145"/>
+    <workbookView xWindow="15210" yWindow="90" windowWidth="13590" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="40">
   <si>
     <t>start application</t>
   </si>
@@ -49,82 +48,100 @@
     <t>port Multimetr</t>
   </si>
   <si>
+    <t>COM4</t>
+  </si>
+  <si>
+    <t>Function linkPort</t>
+  </si>
+  <si>
+    <t>open Port 1</t>
+  </si>
+  <si>
+    <t>COM4:9600,N,8,1</t>
+  </si>
+  <si>
+    <t>request as data and avswer port 1</t>
+  </si>
+  <si>
+    <t>*idn?   GW, GDM8255A, 1.0</t>
+  </si>
+  <si>
+    <t>if length &gt; 0</t>
+  </si>
+  <si>
+    <t>Function multimetrCorrect</t>
+  </si>
+  <si>
+    <t>scan Ports</t>
+  </si>
+  <si>
+    <t>ports() length</t>
+  </si>
+  <si>
+    <t>checkPortsMassive</t>
+  </si>
+  <si>
+    <t>scan Port for A2</t>
+  </si>
+  <si>
+    <t>COM1</t>
+  </si>
+  <si>
+    <t>open Port 2</t>
+  </si>
+  <si>
+    <t>COM1:9600,N,8,1</t>
+  </si>
+  <si>
+    <t>Function sendAngle: anglVar</t>
+  </si>
+  <si>
+    <t>hlo</t>
+  </si>
+  <si>
+    <t>result from Port 2</t>
+  </si>
+  <si>
+    <t>request as data and avswer port 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hlo   </t>
+  </si>
+  <si>
+    <t>else length &gt; 0</t>
+  </si>
+  <si>
+    <t>close Port 2</t>
+  </si>
+  <si>
+    <t>Function controlCorrect</t>
+  </si>
+  <si>
+    <t>portControl hlo = 25</t>
+  </si>
+  <si>
     <t>COM6</t>
   </si>
   <si>
-    <t>Function linkPort</t>
-  </si>
-  <si>
-    <t>open Port 1</t>
-  </si>
-  <si>
     <t>COM6:9600,N,8,1</t>
   </si>
   <si>
-    <t>request as data and avswer port 1</t>
-  </si>
-  <si>
-    <t>*idn?   GW, GDM8255A, 1.0</t>
-  </si>
-  <si>
-    <t>if length &gt; 0</t>
-  </si>
-  <si>
-    <t>Function multimetrCorrect</t>
-  </si>
-  <si>
-    <t>scan Ports</t>
-  </si>
-  <si>
-    <t>ports() length</t>
-  </si>
-  <si>
-    <t>checkPortsMassive</t>
-  </si>
-  <si>
-    <t>scan Port for A2</t>
-  </si>
-  <si>
-    <t>COM1</t>
-  </si>
-  <si>
-    <t>open Port 2</t>
-  </si>
-  <si>
-    <t>COM1:9600,N,8,1</t>
-  </si>
-  <si>
-    <t>Function sendAngle: anglVar</t>
-  </si>
-  <si>
-    <t>hlo</t>
-  </si>
-  <si>
-    <t>result from Port 2</t>
-  </si>
-  <si>
-    <t>request as data and avswer port 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hlo   </t>
-  </si>
-  <si>
-    <t>else length &gt; 0</t>
-  </si>
-  <si>
-    <t>close Port 2</t>
-  </si>
-  <si>
-    <t>Function controlCorrect</t>
-  </si>
-  <si>
-    <t>portControl hlo = 25</t>
+    <t>COM7</t>
+  </si>
+  <si>
+    <t>COM7:9600,N,8,1</t>
+  </si>
+  <si>
+    <t>COM9</t>
+  </si>
+  <si>
+    <t>COM9:9600,N,8,1</t>
   </si>
   <si>
     <t>end checkPortsMassive</t>
   </si>
   <si>
-    <t xml:space="preserve">COM6 </t>
+    <t xml:space="preserve">COM4 </t>
   </si>
   <si>
     <t>close Port 1</t>
@@ -133,8 +150,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,7 +250,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -285,7 +302,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -479,47 +496,47 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>0.59149305555555554</v>
+        <v>0.85703703703703704</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>0.59151620370370372</v>
+        <v>0.85704861111111119</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>0.5915393518518518</v>
+        <v>0.85704861111111119</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -528,9 +545,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>0.59155092592592595</v>
+        <v>0.85706018518518512</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -539,9 +556,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>0.59157407407407414</v>
+        <v>0.85707175925925927</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -550,17 +567,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>0.59159722222222222</v>
+        <v>0.85708333333333331</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>0.59160879629629626</v>
+        <v>0.85709490740740746</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -569,9 +586,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>0.59165509259259264</v>
+        <v>0.85712962962962969</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -580,9 +597,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>0.59167824074074071</v>
+        <v>0.85714120370370372</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -591,9 +608,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>0.59168981481481475</v>
+        <v>0.85715277777777776</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -602,36 +619,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>0.59171296296296294</v>
+        <v>0.85715277777777776</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>0.59173611111111113</v>
+        <v>0.85717592592592595</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>0.59174768518518517</v>
+        <v>0.8571875000000001</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>0.59177083333333336</v>
+        <v>0.85719907407407403</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
@@ -640,17 +657,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>0.59179398148148155</v>
+        <v>0.85721064814814818</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>0.59181712962962962</v>
+        <v>0.85722222222222222</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
@@ -659,9 +676,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>0.59185185185185185</v>
+        <v>0.8572453703703703</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
@@ -670,17 +687,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>0.59187500000000004</v>
+        <v>0.85725694444444445</v>
       </c>
       <c r="B19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>0.59188657407407408</v>
+        <v>0.8572685185185186</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
@@ -689,9 +706,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>0.59190972222222216</v>
+        <v>0.85728009259259252</v>
       </c>
       <c r="B21" t="s">
         <v>27</v>
@@ -700,9 +717,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>0.59193287037037035</v>
+        <v>0.85729166666666667</v>
       </c>
       <c r="B22" t="s">
         <v>28</v>
@@ -711,9 +728,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>0.59195601851851853</v>
+        <v>0.85730324074074071</v>
       </c>
       <c r="B23" t="s">
         <v>29</v>
@@ -722,9 +739,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>0.59197916666666661</v>
+        <v>0.85731481481481486</v>
       </c>
       <c r="B24" t="s">
         <v>30</v>
@@ -733,9 +750,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>0.59199074074074076</v>
+        <v>0.85732638888888879</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
@@ -744,564 +761,800 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>0.59201388888888895</v>
+        <v>0.85739583333333336</v>
       </c>
       <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
         <v>31</v>
       </c>
-      <c r="C26" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>0.85740740740740751</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>0.85741898148148143</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="3">
-        <v>0.59203703703703703</v>
-      </c>
-      <c r="B27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="3">
-        <v>0.59302083333333333</v>
-      </c>
-      <c r="B28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>0.59304398148148152</v>
+        <v>0.85743055555555558</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="3"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="3"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="3"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="3"/>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="3"/>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="3"/>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="3"/>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="3"/>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="3"/>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="3"/>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="3"/>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="3"/>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="3"/>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="3"/>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="3"/>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="3"/>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="3"/>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="3"/>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="3"/>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="3"/>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="3"/>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="3"/>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="3"/>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="3"/>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="3"/>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="3"/>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="3"/>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="3"/>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="3"/>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="3"/>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="3"/>
-    </row>
-    <row r="61" spans="1:1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>0.85744212962962962</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>0.85744212962962962</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>0.85745370370370377</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>0.8574652777777777</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>0.85747685185185185</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>0.857488425925926</v>
+      </c>
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>0.85749999999999993</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>0.85751157407407408</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>0.85752314814814812</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>0.85753472222222227</v>
+      </c>
+      <c r="B39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>0.8575462962962962</v>
+      </c>
+      <c r="B40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>0.85755787037037035</v>
+      </c>
+      <c r="B41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>0.8575694444444445</v>
+      </c>
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>0.85758101851851853</v>
+      </c>
+      <c r="B43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>0.85759259259259257</v>
+      </c>
+      <c r="B44" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>0.85760416666666661</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>0.85761574074074076</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>0.85762731481481491</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>0.85762731481481491</v>
+      </c>
+      <c r="B48" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>0.85766203703703703</v>
+      </c>
+      <c r="B49" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>0.85767361111111118</v>
+      </c>
+      <c r="B50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>0.85768518518518511</v>
+      </c>
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>0.85769675925925926</v>
+      </c>
+      <c r="B52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>0.85770833333333341</v>
+      </c>
+      <c r="B53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>0.85770833333333341</v>
+      </c>
+      <c r="B54" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>0.85771990740740733</v>
+      </c>
+      <c r="B55" t="s">
+        <v>30</v>
+      </c>
+      <c r="C55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>0.85773148148148148</v>
+      </c>
+      <c r="B56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>0.85774305555555552</v>
+      </c>
+      <c r="B57" t="s">
+        <v>37</v>
+      </c>
+      <c r="C57" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>0.85775462962962967</v>
+      </c>
+      <c r="B58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>0.85787037037037039</v>
+      </c>
+      <c r="B59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>0.85787037037037039</v>
+      </c>
+      <c r="B60" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="3"/>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="3"/>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="3"/>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="3"/>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="3"/>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="3"/>
     </row>
-    <row r="162" spans="1:1">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="3"/>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="3"/>
     </row>
-    <row r="164" spans="1:1">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="3"/>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
     </row>
-    <row r="166" spans="1:1">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="3"/>
     </row>
-    <row r="167" spans="1:1">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="3"/>
     </row>
-    <row r="168" spans="1:1">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="3"/>
     </row>
-    <row r="169" spans="1:1">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="3"/>
     </row>
-    <row r="170" spans="1:1">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="3"/>
     </row>
-    <row r="171" spans="1:1">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="3"/>
     </row>
-    <row r="172" spans="1:1">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="3"/>
     </row>
-    <row r="173" spans="1:1">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="3"/>
     </row>
-    <row r="174" spans="1:1">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="3"/>
     </row>
-    <row r="175" spans="1:1">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="3"/>
     </row>
-    <row r="176" spans="1:1">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
     </row>
-    <row r="177" spans="1:1">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="3"/>
     </row>
-    <row r="178" spans="1:1">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="3"/>
     </row>
-    <row r="179" spans="1:1">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="3"/>
     </row>
-    <row r="180" spans="1:1">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="3"/>
     </row>
-    <row r="181" spans="1:1">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="3"/>
     </row>
-    <row r="182" spans="1:1">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="3"/>
     </row>
-    <row r="183" spans="1:1">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="3"/>
     </row>
-    <row r="184" spans="1:1">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="3"/>
     </row>
-    <row r="185" spans="1:1">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="3"/>
     </row>
-    <row r="186" spans="1:1">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="3"/>
     </row>
-    <row r="187" spans="1:1">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="3"/>
     </row>
-    <row r="188" spans="1:1">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="3"/>
     </row>
-    <row r="189" spans="1:1">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="3"/>
     </row>
-    <row r="190" spans="1:1">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="3"/>
     </row>
-    <row r="191" spans="1:1">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="3"/>
     </row>
-    <row r="192" spans="1:1">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="3"/>
     </row>
-    <row r="193" spans="1:1">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="3"/>
     </row>
-    <row r="194" spans="1:1">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="3"/>
     </row>
-    <row r="195" spans="1:1">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="3"/>
     </row>
-    <row r="196" spans="1:1">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="3"/>
     </row>
-    <row r="197" spans="1:1">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="3"/>
     </row>
-    <row r="198" spans="1:1">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="3"/>
     </row>
-    <row r="199" spans="1:1">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="3"/>
     </row>
-    <row r="200" spans="1:1">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="3"/>
     </row>
-    <row r="201" spans="1:1">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add method for rotating to zero
</commit_message>
<xml_diff>
--- a/applications/VBA/logLine.xlsx
+++ b/applications/VBA/logLine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\Linearity\applications\VBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED773AA-B3B7-4118-9DA8-AC9E4ED64F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC95FDCF-B222-4B49-BF44-7372C3B16D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15210" yWindow="90" windowWidth="13590" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>start application</t>
   </si>
@@ -48,7 +48,22 @@
     <t>port Multimetr</t>
   </si>
   <si>
-    <t>COM4</t>
+    <t>port Control</t>
+  </si>
+  <si>
+    <t>scan Ports</t>
+  </si>
+  <si>
+    <t>ports() length</t>
+  </si>
+  <si>
+    <t>checkPortsMassive</t>
+  </si>
+  <si>
+    <t>scan Port for A1</t>
+  </si>
+  <si>
+    <t>COM1</t>
   </si>
   <si>
     <t>Function linkPort</t>
@@ -57,94 +72,7 @@
     <t>open Port 1</t>
   </si>
   <si>
-    <t>COM4:9600,N,8,1</t>
-  </si>
-  <si>
-    <t>request as data and avswer port 1</t>
-  </si>
-  <si>
-    <t>*idn?   GW, GDM8255A, 1.0</t>
-  </si>
-  <si>
-    <t>if length &gt; 0</t>
-  </si>
-  <si>
-    <t>Function multimetrCorrect</t>
-  </si>
-  <si>
-    <t>scan Ports</t>
-  </si>
-  <si>
-    <t>ports() length</t>
-  </si>
-  <si>
-    <t>checkPortsMassive</t>
-  </si>
-  <si>
-    <t>scan Port for A2</t>
-  </si>
-  <si>
-    <t>COM1</t>
-  </si>
-  <si>
-    <t>open Port 2</t>
-  </si>
-  <si>
     <t>COM1:9600,N,8,1</t>
-  </si>
-  <si>
-    <t>Function sendAngle: anglVar</t>
-  </si>
-  <si>
-    <t>hlo</t>
-  </si>
-  <si>
-    <t>result from Port 2</t>
-  </si>
-  <si>
-    <t>request as data and avswer port 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hlo   </t>
-  </si>
-  <si>
-    <t>else length &gt; 0</t>
-  </si>
-  <si>
-    <t>close Port 2</t>
-  </si>
-  <si>
-    <t>Function controlCorrect</t>
-  </si>
-  <si>
-    <t>portControl hlo = 25</t>
-  </si>
-  <si>
-    <t>COM6</t>
-  </si>
-  <si>
-    <t>COM6:9600,N,8,1</t>
-  </si>
-  <si>
-    <t>COM7</t>
-  </si>
-  <si>
-    <t>COM7:9600,N,8,1</t>
-  </si>
-  <si>
-    <t>COM9</t>
-  </si>
-  <si>
-    <t>COM9:9600,N,8,1</t>
-  </si>
-  <si>
-    <t>end checkPortsMassive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COM4 </t>
-  </si>
-  <si>
-    <t>close Port 1</t>
   </si>
 </sst>
 </file>
@@ -181,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -190,6 +118,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -520,7 +451,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>0.85703703703703704</v>
+        <v>0.77612268518518512</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -528,7 +459,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>0.85704861111111119</v>
+        <v>0.77613425925925927</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -536,7 +467,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>0.85704861111111119</v>
+        <v>0.77614583333333342</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -547,7 +478,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>0.85706018518518512</v>
+        <v>0.77615740740740735</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -558,592 +489,230 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>0.85707175925925927</v>
+        <v>0.77615740740740735</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>0.85708333333333331</v>
+        <v>0.7761689814814815</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>0.85709490740740746</v>
+        <v>0.77618055555555554</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>0.85712962962962969</v>
+        <v>0.77619212962962969</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>0.85714120370370372</v>
+        <v>0.77620370370370362</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>0.85715277777777776</v>
+        <v>0.77621527777777777</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="b">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>0.85715277777777776</v>
+        <v>0.77622685185185192</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>0.85717592592592595</v>
+        <v>0.77623842592592596</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>0.8571875000000001</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
+      <c r="A14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>0.85719907407407403</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
+      <c r="A15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>0.85721064814814818</v>
-      </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>0.85722222222222222</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>0.8572453703703703</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>0.85725694444444445</v>
-      </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>0.8572685185185186</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>0.85728009259259252</v>
-      </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>0.85729166666666667</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>0.85730324074074071</v>
-      </c>
-      <c r="B23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>0.85731481481481486</v>
-      </c>
-      <c r="B24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>0.85732638888888879</v>
-      </c>
-      <c r="B25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>0.85739583333333336</v>
-      </c>
-      <c r="B26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>0.85740740740740751</v>
-      </c>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>0.85741898148148143</v>
-      </c>
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>0.85743055555555558</v>
-      </c>
-      <c r="B29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>0.85744212962962962</v>
-      </c>
-      <c r="B30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>0.85744212962962962</v>
-      </c>
-      <c r="B31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>0.85745370370370377</v>
-      </c>
-      <c r="B32" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" t="s">
-        <v>32</v>
-      </c>
+      <c r="A16" s="3"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>0.8574652777777777</v>
-      </c>
-      <c r="B33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" t="b">
-        <v>0</v>
-      </c>
+      <c r="A33" s="3"/>
+      <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>0.85747685185185185</v>
-      </c>
-      <c r="B34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" t="b">
-        <v>0</v>
-      </c>
+      <c r="A34" s="3"/>
+      <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>0.857488425925926</v>
-      </c>
-      <c r="B35" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" t="s">
-        <v>32</v>
-      </c>
+      <c r="A35" s="3"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>0.85749999999999993</v>
-      </c>
-      <c r="B36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C36" t="s">
-        <v>33</v>
-      </c>
+      <c r="A36" s="3"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>0.85751157407407408</v>
-      </c>
-      <c r="B37" t="s">
-        <v>8</v>
-      </c>
+      <c r="A37" s="3"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>0.85752314814814812</v>
-      </c>
-      <c r="B38" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" t="s">
-        <v>34</v>
-      </c>
+      <c r="A38" s="3"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
-        <v>0.85753472222222227</v>
-      </c>
-      <c r="B39" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" t="s">
-        <v>34</v>
-      </c>
+      <c r="A39" s="3"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>0.8575462962962962</v>
-      </c>
-      <c r="B40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" t="s">
-        <v>26</v>
-      </c>
+      <c r="A40" s="3"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <v>0.85755787037037035</v>
-      </c>
-      <c r="B41" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
+      <c r="A41" s="3"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
-        <v>0.8575694444444445</v>
-      </c>
-      <c r="B42" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" t="s">
-        <v>34</v>
-      </c>
+      <c r="A42" s="3"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
-        <v>0.85758101851851853</v>
-      </c>
-      <c r="B43" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" t="b">
-        <v>0</v>
-      </c>
+      <c r="A43" s="3"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
-        <v>0.85759259259259257</v>
-      </c>
-      <c r="B44" t="s">
-        <v>30</v>
-      </c>
-      <c r="C44" t="b">
-        <v>0</v>
-      </c>
+      <c r="A44" s="3"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
-        <v>0.85760416666666661</v>
-      </c>
-      <c r="B45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45" t="s">
-        <v>34</v>
-      </c>
+      <c r="A45" s="3"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>0.85761574074074076</v>
-      </c>
-      <c r="B46" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46" t="s">
-        <v>35</v>
-      </c>
+      <c r="A46" s="3"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>0.85762731481481491</v>
-      </c>
-      <c r="B47" t="s">
-        <v>8</v>
-      </c>
+      <c r="A47" s="3"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
-        <v>0.85762731481481491</v>
-      </c>
-      <c r="B48" t="s">
-        <v>20</v>
-      </c>
-      <c r="C48" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
-        <v>0.85766203703703703</v>
-      </c>
-      <c r="B49" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
-        <v>0.85767361111111118</v>
-      </c>
-      <c r="B50" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="3">
-        <v>0.85768518518518511</v>
-      </c>
-      <c r="B51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C51" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
-        <v>0.85769675925925926</v>
-      </c>
-      <c r="B52" t="s">
-        <v>27</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="3">
-        <v>0.85770833333333341</v>
-      </c>
-      <c r="B53" t="s">
-        <v>28</v>
-      </c>
-      <c r="C53" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
-        <v>0.85770833333333341</v>
-      </c>
-      <c r="B54" t="s">
-        <v>29</v>
-      </c>
-      <c r="C54" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="3">
-        <v>0.85771990740740733</v>
-      </c>
-      <c r="B55" t="s">
-        <v>30</v>
-      </c>
-      <c r="C55" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="3">
-        <v>0.85773148148148148</v>
-      </c>
-      <c r="B56" t="s">
-        <v>28</v>
-      </c>
-      <c r="C56" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="3">
-        <v>0.85774305555555552</v>
-      </c>
-      <c r="B57" t="s">
-        <v>37</v>
-      </c>
-      <c r="C57" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="3">
-        <v>0.85775462962962967</v>
-      </c>
-      <c r="B58" t="s">
-        <v>28</v>
-      </c>
-      <c r="C58" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="3">
-        <v>0.85787037037037039</v>
-      </c>
-      <c r="B59" t="s">
-        <v>39</v>
-      </c>
-      <c r="C59" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="3">
-        <v>0.85787037037037039</v>
-      </c>
-      <c r="B60" t="s">
-        <v>28</v>
-      </c>
-      <c r="C60" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
@@ -1338,148 +907,154 @@
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C138" s="4"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C139" s="4"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="3"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C152" s="4"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C153" s="4"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="3"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="3"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="3"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="3"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="3"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="3"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="3"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="3"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="3"/>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C166" s="4"/>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="3"/>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C167" s="4"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="3"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="3"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="3"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="3"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="3"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="3"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="3"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="3"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>